<commit_message>
Added 7-segment driver and adapter requirements, pending review
</commit_message>
<xml_diff>
--- a/Documentation/Stopwatch_Project_Schedule.xlsx
+++ b/Documentation/Stopwatch_Project_Schedule.xlsx
@@ -5,24 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djste\Documents\GitHub\Time_Travelers_Verilog_Stopwatch\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Files\LTTS\FPGA Training\Projects\Verilog\StopWatch_Verilog\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63DE928A-5A2A-4F46-8B38-E79E88DBE9AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADFA585-B88F-4635-8D55-02ABE5B47CE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="77">
   <si>
     <t>Project Stage</t>
   </si>
@@ -258,6 +256,9 @@
   </si>
   <si>
     <t>Debrief</t>
+  </si>
+  <si>
+    <t>HR mandatory training</t>
   </si>
 </sst>
 </file>
@@ -332,7 +333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -603,11 +604,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -704,9 +748,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -717,34 +775,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1063,26 +1112,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="46" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="34.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" customWidth="1"/>
+    <col min="10" max="10" width="34.109375" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -1114,8 +1163,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="63" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="50" t="s">
@@ -1140,8 +1189,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="68"/>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="71"/>
       <c r="B3" s="51" t="s">
         <v>15</v>
       </c>
@@ -1151,10 +1200,10 @@
       <c r="D3" s="48" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="76">
+      <c r="E3" s="62">
         <v>43991</v>
       </c>
-      <c r="F3" s="70">
+      <c r="F3" s="66">
         <v>43986</v>
       </c>
       <c r="G3" s="59" t="s">
@@ -1166,8 +1215,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="68"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="71"/>
       <c r="B4" s="51" t="s">
         <v>20</v>
       </c>
@@ -1180,7 +1229,7 @@
       <c r="E4" s="36">
         <v>43986</v>
       </c>
-      <c r="F4" s="70"/>
+      <c r="F4" s="66"/>
       <c r="G4" s="60"/>
       <c r="H4" s="25"/>
       <c r="I4" s="10"/>
@@ -1188,8 +1237,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="68"/>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="71"/>
       <c r="B5" s="51" t="s">
         <v>23</v>
       </c>
@@ -1212,8 +1261,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="68"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="71"/>
       <c r="B6" s="51" t="s">
         <v>26</v>
       </c>
@@ -1234,8 +1283,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="69"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="64"/>
       <c r="B7" s="52" t="s">
         <v>24</v>
       </c>
@@ -1252,8 +1301,8 @@
       <c r="I7" s="11"/>
       <c r="J7" s="11"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="64" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="68" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="50" t="s">
@@ -1262,13 +1311,13 @@
       <c r="C8" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="71" t="s">
+      <c r="D8" s="72" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="39">
         <v>43987</v>
       </c>
-      <c r="F8" s="73">
+      <c r="F8" s="65">
         <v>43990</v>
       </c>
       <c r="G8" s="24"/>
@@ -1276,26 +1325,26 @@
       <c r="I8" s="16"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="65"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="69"/>
       <c r="B9" s="53" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="72"/>
+      <c r="D9" s="73"/>
       <c r="E9" s="40">
         <v>43987</v>
       </c>
-      <c r="F9" s="70"/>
-      <c r="G9" s="25"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="76"/>
       <c r="H9" s="25"/>
       <c r="I9" s="10"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="65"/>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="69"/>
       <c r="B10" s="53" t="s">
         <v>34</v>
       </c>
@@ -1303,15 +1352,17 @@
         <v>35</v>
       </c>
       <c r="D10" s="48"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="25"/>
+      <c r="E10" s="79">
+        <v>43990</v>
+      </c>
+      <c r="F10" s="66"/>
+      <c r="G10" s="77"/>
       <c r="H10" s="25"/>
       <c r="I10" s="10"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="66"/>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="70"/>
       <c r="B11" s="54" t="s">
         <v>36</v>
       </c>
@@ -1319,19 +1370,23 @@
         <v>12</v>
       </c>
       <c r="D11" s="49"/>
-      <c r="E11" s="63"/>
+      <c r="E11" s="78">
+        <v>43993</v>
+      </c>
       <c r="F11" s="34">
         <v>43992</v>
       </c>
-      <c r="G11" s="26"/>
+      <c r="G11" s="75" t="s">
+        <v>76</v>
+      </c>
       <c r="H11" s="26"/>
       <c r="I11" s="11"/>
       <c r="J11" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="67" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="63" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="55" t="s">
@@ -1344,7 +1399,7 @@
         <v>41</v>
       </c>
       <c r="E12" s="42"/>
-      <c r="F12" s="73">
+      <c r="F12" s="65">
         <v>43993</v>
       </c>
       <c r="G12" s="24"/>
@@ -1354,8 +1409,8 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="68"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="71"/>
       <c r="B13" s="53" t="s">
         <v>43</v>
       </c>
@@ -1366,7 +1421,7 @@
         <v>41</v>
       </c>
       <c r="E13" s="43"/>
-      <c r="F13" s="70"/>
+      <c r="F13" s="66"/>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
       <c r="I13" s="10"/>
@@ -1374,8 +1429,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="68"/>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="71"/>
       <c r="B14" s="53" t="s">
         <v>46</v>
       </c>
@@ -1386,7 +1441,7 @@
         <v>41</v>
       </c>
       <c r="E14" s="43"/>
-      <c r="F14" s="70"/>
+      <c r="F14" s="66"/>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
       <c r="I14" s="10"/>
@@ -1394,8 +1449,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="69"/>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="64"/>
       <c r="B15" s="54" t="s">
         <v>48</v>
       </c>
@@ -1406,7 +1461,7 @@
         <v>41</v>
       </c>
       <c r="E15" s="44"/>
-      <c r="F15" s="70"/>
+      <c r="F15" s="66"/>
       <c r="G15" s="26"/>
       <c r="H15" s="26"/>
       <c r="I15" s="11"/>
@@ -1414,8 +1469,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="68" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="50" t="s">
@@ -1426,15 +1481,15 @@
       </c>
       <c r="D16" s="47"/>
       <c r="E16" s="42"/>
-      <c r="F16" s="73">
+      <c r="F16" s="65">
         <v>43994</v>
       </c>
       <c r="G16" s="24"/>
       <c r="H16" s="24"/>
       <c r="I16" s="16"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="69"/>
       <c r="B17" s="51" t="s">
         <v>53</v>
       </c>
@@ -1443,13 +1498,13 @@
       </c>
       <c r="D17" s="48"/>
       <c r="E17" s="43"/>
-      <c r="F17" s="70"/>
+      <c r="F17" s="66"/>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
       <c r="I17" s="10"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="65"/>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="69"/>
       <c r="B18" s="51" t="s">
         <v>54</v>
       </c>
@@ -1458,13 +1513,13 @@
       </c>
       <c r="D18" s="48"/>
       <c r="E18" s="43"/>
-      <c r="F18" s="70"/>
+      <c r="F18" s="66"/>
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="66"/>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="70"/>
       <c r="B19" s="52" t="s">
         <v>55</v>
       </c>
@@ -1473,13 +1528,13 @@
       </c>
       <c r="D19" s="49"/>
       <c r="E19" s="44"/>
-      <c r="F19" s="70"/>
+      <c r="F19" s="66"/>
       <c r="G19" s="26"/>
       <c r="H19" s="26"/>
       <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="64" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="68" t="s">
         <v>56</v>
       </c>
       <c r="B20" s="55" t="s">
@@ -1490,15 +1545,15 @@
       </c>
       <c r="D20" s="47"/>
       <c r="E20" s="42"/>
-      <c r="F20" s="73">
+      <c r="F20" s="65">
         <v>43997</v>
       </c>
       <c r="G20" s="24"/>
       <c r="H20" s="24"/>
       <c r="I20" s="16"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="65"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="69"/>
       <c r="B21" s="53" t="s">
         <v>58</v>
       </c>
@@ -1507,13 +1562,13 @@
       </c>
       <c r="D21" s="48"/>
       <c r="E21" s="43"/>
-      <c r="F21" s="70"/>
+      <c r="F21" s="66"/>
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="65"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="69"/>
       <c r="B22" s="53" t="s">
         <v>59</v>
       </c>
@@ -1522,13 +1577,13 @@
       </c>
       <c r="D22" s="48"/>
       <c r="E22" s="43"/>
-      <c r="F22" s="70"/>
+      <c r="F22" s="66"/>
       <c r="G22" s="25"/>
       <c r="H22" s="25"/>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="65"/>
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="69"/>
       <c r="B23" s="53" t="s">
         <v>60</v>
       </c>
@@ -1537,13 +1592,13 @@
       </c>
       <c r="D23" s="48"/>
       <c r="E23" s="43"/>
-      <c r="F23" s="75"/>
+      <c r="F23" s="67"/>
       <c r="G23" s="25"/>
       <c r="H23" s="25"/>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="65"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="69"/>
       <c r="B24" s="53" t="s">
         <v>61</v>
       </c>
@@ -1552,15 +1607,15 @@
       </c>
       <c r="D24" s="48"/>
       <c r="E24" s="43"/>
-      <c r="F24" s="70">
+      <c r="F24" s="66">
         <v>43998</v>
       </c>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="65"/>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="69"/>
       <c r="B25" s="53" t="s">
         <v>53</v>
       </c>
@@ -1569,13 +1624,13 @@
       </c>
       <c r="D25" s="48"/>
       <c r="E25" s="43"/>
-      <c r="F25" s="70"/>
+      <c r="F25" s="66"/>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="65"/>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="69"/>
       <c r="B26" s="53" t="s">
         <v>62</v>
       </c>
@@ -1584,13 +1639,13 @@
       </c>
       <c r="D26" s="48"/>
       <c r="E26" s="43"/>
-      <c r="F26" s="70"/>
+      <c r="F26" s="66"/>
       <c r="G26" s="25"/>
       <c r="H26" s="25"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="66"/>
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="70"/>
       <c r="B27" s="54" t="s">
         <v>63</v>
       </c>
@@ -1599,12 +1654,12 @@
       </c>
       <c r="D27" s="49"/>
       <c r="E27" s="45"/>
-      <c r="F27" s="75"/>
+      <c r="F27" s="67"/>
       <c r="G27" s="26"/>
       <c r="H27" s="26"/>
       <c r="I27" s="11"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="32" t="s">
         <v>64</v>
       </c>
@@ -1616,15 +1671,15 @@
       </c>
       <c r="D28" s="27"/>
       <c r="E28" s="29"/>
-      <c r="F28" s="73">
+      <c r="F28" s="65">
         <v>43999</v>
       </c>
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="67" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="63" t="s">
         <v>66</v>
       </c>
       <c r="B29" s="55" t="s">
@@ -1635,13 +1690,13 @@
       </c>
       <c r="D29" s="47"/>
       <c r="E29" s="46"/>
-      <c r="F29" s="70"/>
+      <c r="F29" s="66"/>
       <c r="G29" s="24"/>
       <c r="H29" s="24"/>
       <c r="I29" s="16"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="69"/>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="64"/>
       <c r="B30" s="52" t="s">
         <v>68</v>
       </c>
@@ -1650,13 +1705,13 @@
       </c>
       <c r="D30" s="49"/>
       <c r="E30" s="45"/>
-      <c r="F30" s="70"/>
+      <c r="F30" s="66"/>
       <c r="G30" s="26"/>
       <c r="H30" s="26"/>
       <c r="I30" s="11"/>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="64" t="s">
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="68" t="s">
         <v>69</v>
       </c>
       <c r="B31" s="56" t="s">
@@ -1667,13 +1722,13 @@
       </c>
       <c r="D31" s="47"/>
       <c r="E31" s="46"/>
-      <c r="F31" s="75"/>
+      <c r="F31" s="67"/>
       <c r="G31" s="24"/>
       <c r="H31" s="24"/>
       <c r="I31" s="16"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="65"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="69"/>
       <c r="B32" s="53" t="s">
         <v>71</v>
       </c>
@@ -1682,15 +1737,15 @@
       </c>
       <c r="D32" s="48"/>
       <c r="E32" s="43"/>
-      <c r="F32" s="70">
+      <c r="F32" s="66">
         <v>44000</v>
       </c>
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="66"/>
+    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="70"/>
       <c r="B33" s="52" t="s">
         <v>72</v>
       </c>
@@ -1699,13 +1754,13 @@
       </c>
       <c r="D33" s="49"/>
       <c r="E33" s="45"/>
-      <c r="F33" s="70"/>
+      <c r="F33" s="66"/>
       <c r="G33" s="26"/>
       <c r="H33" s="26"/>
       <c r="I33" s="11"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="67" t="s">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="63" t="s">
         <v>73</v>
       </c>
       <c r="B34" s="55" t="s">
@@ -1716,14 +1771,14 @@
       </c>
       <c r="D34" s="47"/>
       <c r="E34" s="46"/>
-      <c r="F34" s="70"/>
+      <c r="F34" s="66"/>
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
       <c r="I34" s="10"/>
       <c r="L34" s="6"/>
     </row>
-    <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="69"/>
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="64"/>
       <c r="B35" s="54" t="s">
         <v>75</v>
       </c>
@@ -1732,12 +1787,12 @@
       </c>
       <c r="D35" s="49"/>
       <c r="E35" s="45"/>
-      <c r="F35" s="75"/>
+      <c r="F35" s="67"/>
       <c r="G35" s="26"/>
       <c r="H35" s="26"/>
       <c r="I35" s="11"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="9"/>
@@ -1747,23 +1802,15 @@
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B37" s="6"/>
     </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E51" s="5"/>
       <c r="F51" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="A20:A27"/>
     <mergeCell ref="A16:A19"/>
     <mergeCell ref="A12:A15"/>
     <mergeCell ref="A8:A11"/>
@@ -1774,12 +1821,35 @@
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="F12:F15"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="F20:F23"/>
+    <mergeCell ref="F24:F27"/>
+    <mergeCell ref="A31:A33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="F28:F31"/>
+    <mergeCell ref="A20:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="291a90324d5b7e405cdee1cca19d0e54">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a3d94df2e09d7482e07420c2cba8fd2" ns2:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -1925,22 +1995,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{284D3BA3-53DF-4CD6-A7BE-83F88846B803}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E4F7A1-BDD0-42E0-BF8D-BCF9AB8D9DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E8BDE2A-513D-413D-BAAB-708A15D461DA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1956,21 +2028,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E4F7A1-BDD0-42E0-BF8D-BCF9AB8D9DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{284D3BA3-53DF-4CD6-A7BE-83F88846B803}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update to Project Schedule
Added granularity to accomodate Jira ticket tracking.
</commit_message>
<xml_diff>
--- a/Documentation/Stopwatch_Project_Schedule.xlsx
+++ b/Documentation/Stopwatch_Project_Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djste\Documents\GitHub\Time_Travelers_Verilog_Stopwatch\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F99EDA-F5AC-4CDA-90C4-E8B21E3DCEA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5112992E-B82C-4B14-AAC4-DD2C75DD1C55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
   <si>
     <t>Project Stage</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Reason for Delay</t>
   </si>
   <si>
-    <t>Action Taken</t>
-  </si>
-  <si>
     <t>Git Commit tag</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
     <t>Antonio</t>
   </si>
   <si>
-    <t>Reviewed by:</t>
-  </si>
-  <si>
     <t>Team Lead: Waseem</t>
   </si>
   <si>
@@ -171,9 +165,6 @@
     <t>Verilog Expert: Antonio</t>
   </si>
   <si>
-    <t>7-Segment Display Requirements</t>
-  </si>
-  <si>
     <t>Waseem</t>
   </si>
   <si>
@@ -204,9 +195,6 @@
     <t>10 ms Timer Test Bench</t>
   </si>
   <si>
-    <t>20-bit Decimal Up Counter Test Bench</t>
-  </si>
-  <si>
     <t>7-Segment Display Module Test Bench</t>
   </si>
   <si>
@@ -262,6 +250,103 @@
   </si>
   <si>
     <t>7e5e145</t>
+  </si>
+  <si>
+    <t>e02e6e4</t>
+  </si>
+  <si>
+    <t>22e413f</t>
+  </si>
+  <si>
+    <t>Reviewed by: Harry</t>
+  </si>
+  <si>
+    <t>Reviewed by: Devon</t>
+  </si>
+  <si>
+    <t>Reviewed by: Waseem</t>
+  </si>
+  <si>
+    <t>Reviewed by: Antonio</t>
+  </si>
+  <si>
+    <t>Github merging issues. Formatting discrepancies not addressed in standards.</t>
+  </si>
+  <si>
+    <t>7-Segment Driver Requirements</t>
+  </si>
+  <si>
+    <t>7-Segment Adapter Requirements</t>
+  </si>
+  <si>
+    <t>General Requirements</t>
+  </si>
+  <si>
+    <t>7 Segment Adapter Module</t>
+  </si>
+  <si>
+    <t>Trigger Detection Test Cases</t>
+  </si>
+  <si>
+    <t>10 ms Timer Test Cases</t>
+  </si>
+  <si>
+    <t>7-Segment Display Module Test Cases</t>
+  </si>
+  <si>
+    <t>24-bit Counter Test Bench</t>
+  </si>
+  <si>
+    <t>24-bit Counter Test Cases</t>
+  </si>
+  <si>
+    <t>Jira Ticket</t>
+  </si>
+  <si>
+    <t>SWATCH1-101, 102, 103, 104</t>
+  </si>
+  <si>
+    <t>SWATCH1-105, 106, 107, 108</t>
+  </si>
+  <si>
+    <t>SWATCH1-140</t>
+  </si>
+  <si>
+    <t>SWATCH1-53</t>
+  </si>
+  <si>
+    <t>SWATCH1-26</t>
+  </si>
+  <si>
+    <t>SWATCH1-56</t>
+  </si>
+  <si>
+    <t>SWATCH1-142</t>
+  </si>
+  <si>
+    <t>SWATCH1-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A
+</t>
+  </si>
+  <si>
+    <t>SWATCH1-141, 145</t>
+  </si>
+  <si>
+    <t>SWATCH1-115, 116</t>
+  </si>
+  <si>
+    <t>SWATCH1-117, 118</t>
+  </si>
+  <si>
+    <t>SWATCH1-113, 114</t>
+  </si>
+  <si>
+    <t>SWATCH1-111, 112</t>
+  </si>
+  <si>
+    <t>SWATCH1-109, 110</t>
   </si>
 </sst>
 </file>
@@ -343,7 +428,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -657,11 +742,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -770,6 +864,30 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -779,40 +897,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1129,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1291,7 @@
     <col min="5" max="5" width="20.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="46" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" customWidth="1"/>
     <col min="10" max="10" width="34.140625" customWidth="1"/>
     <col min="11" max="11" width="17.140625" customWidth="1"/>
@@ -1173,24 +1320,24 @@
         <v>6</v>
       </c>
       <c r="H1" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="C2" s="47" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="47" t="s">
-        <v>12</v>
       </c>
       <c r="D2" s="47"/>
       <c r="E2" s="35">
@@ -1200,24 +1347,26 @@
         <v>43985</v>
       </c>
       <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="80" t="s">
-        <v>76</v>
+      <c r="H2" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="I2" s="68" t="s">
+        <v>72</v>
       </c>
       <c r="J2" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="79"/>
+      <c r="B3" s="51" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="72"/>
-      <c r="B3" s="51" t="s">
+      <c r="C3" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="D3" s="48" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" s="48" t="s">
-        <v>16</v>
       </c>
       <c r="E3" s="62">
         <v>43991</v>
@@ -1226,153 +1375,155 @@
         <v>43986</v>
       </c>
       <c r="G3" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="88"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="19" t="s">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="79"/>
+      <c r="B4" s="51" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="72"/>
-      <c r="B4" s="51" t="s">
+      <c r="C4" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="48" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>20</v>
       </c>
       <c r="E4" s="36">
         <v>43986</v>
       </c>
       <c r="F4" s="74"/>
       <c r="G4" s="60"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="81" t="s">
-        <v>77</v>
+      <c r="H4" s="88"/>
+      <c r="I4" s="69" t="s">
+        <v>73</v>
       </c>
       <c r="J4" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="79"/>
+      <c r="B5" s="51" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="72"/>
-      <c r="B5" s="51" t="s">
-        <v>22</v>
-      </c>
       <c r="C5" s="48" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="48"/>
       <c r="E5" s="37">
         <v>43990</v>
       </c>
-      <c r="F5" s="78">
+      <c r="F5" s="82">
         <v>43987</v>
       </c>
       <c r="G5" s="60" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="88"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="25"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="21" t="s">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="79"/>
+      <c r="B6" s="51" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
-      <c r="B6" s="51" t="s">
+      <c r="C6" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="48" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="48" t="s">
-        <v>26</v>
       </c>
       <c r="E6" s="36">
         <v>43987</v>
       </c>
-      <c r="F6" s="78"/>
+      <c r="F6" s="82"/>
       <c r="G6" s="60"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="81"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="69"/>
       <c r="J6" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="73"/>
+      <c r="A7" s="72"/>
       <c r="B7" s="52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="49"/>
       <c r="D7" s="49"/>
       <c r="E7" s="38">
         <v>43990</v>
       </c>
-      <c r="F7" s="78"/>
+      <c r="F7" s="82"/>
       <c r="G7" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="89"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="11"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="68" t="s">
+      <c r="B8" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="C8" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="80" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="75" t="s">
-        <v>31</v>
       </c>
       <c r="E8" s="39">
         <v>43987</v>
       </c>
-      <c r="F8" s="77">
+      <c r="F8" s="73">
         <v>43990</v>
       </c>
       <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="80" t="s">
-        <v>77</v>
+      <c r="H8" s="98"/>
+      <c r="I8" s="68" t="s">
+        <v>74</v>
       </c>
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="69"/>
+      <c r="A9" s="77"/>
       <c r="B9" s="53" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="76"/>
+        <v>11</v>
+      </c>
+      <c r="D9" s="81"/>
       <c r="E9" s="40">
         <v>43987</v>
       </c>
       <c r="F9" s="74"/>
       <c r="G9" s="64"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="81"/>
+      <c r="H9" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" s="69"/>
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="69"/>
+      <c r="A10" s="77"/>
       <c r="B10" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="48" t="s">
         <v>33</v>
-      </c>
-      <c r="C10" s="48" t="s">
-        <v>34</v>
       </c>
       <c r="D10" s="48"/>
       <c r="E10" s="67">
@@ -1380,17 +1531,19 @@
       </c>
       <c r="F10" s="74"/>
       <c r="G10" s="65"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="81"/>
+      <c r="H10" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" s="69"/>
       <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="70"/>
+      <c r="A11" s="78"/>
       <c r="B11" s="54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" s="49"/>
       <c r="E11" s="66">
@@ -1400,461 +1553,604 @@
         <v>43992</v>
       </c>
       <c r="G11" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" s="26"/>
+        <v>71</v>
+      </c>
+      <c r="H11" s="26" t="s">
+        <v>92</v>
+      </c>
       <c r="I11" s="11"/>
       <c r="J11" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="71" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="90">
+        <v>43994</v>
+      </c>
+      <c r="F12" s="73">
+        <v>43993</v>
+      </c>
+      <c r="G12" s="87" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="I12" s="86" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="79"/>
+      <c r="B13" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="C13" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="47" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="47" t="s">
+      <c r="D13" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="E13" s="91"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="88"/>
+      <c r="H13" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="I13" s="84"/>
+      <c r="J13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="79"/>
+      <c r="B14" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="42"/>
-      <c r="F12" s="77">
-        <v>43993</v>
-      </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="3" t="s">
+      <c r="C14" s="48" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="72"/>
-      <c r="B13" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="48" t="s">
+      <c r="D14" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="91"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="84"/>
+      <c r="J14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="79"/>
+      <c r="B15" s="53" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="43"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="10"/>
-      <c r="J13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="72"/>
-      <c r="B14" s="53" t="s">
+      <c r="C15" s="94" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="94" t="s">
+        <v>78</v>
+      </c>
+      <c r="E15" s="91"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="88"/>
+      <c r="H15" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I15" s="84"/>
+      <c r="J15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="79"/>
+      <c r="B16" s="93" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="10"/>
-      <c r="J14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="73"/>
-      <c r="B15" s="54" t="s">
+      <c r="D16" s="94" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="91"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="88"/>
+      <c r="H16" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" s="84"/>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="72"/>
+      <c r="B17" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="92"/>
+      <c r="F17" s="74"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" s="85"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="49" t="s">
+      <c r="B18" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="11"/>
-      <c r="J15" t="s">
+      <c r="C18" s="57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="47"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="73">
+        <v>43994</v>
+      </c>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="I18" s="16"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="77"/>
+      <c r="B19" s="51" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
+      <c r="C19" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="74"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="77"/>
+      <c r="B20" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="77">
-        <v>43994</v>
-      </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="16"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="69"/>
-      <c r="B17" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="48"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="10"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="69"/>
-      <c r="B18" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="48"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="10"/>
-    </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="70"/>
-      <c r="B19" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="C19" s="58" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="49"/>
-      <c r="E19" s="44"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="68" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="55" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="57" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="47"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="77">
-        <v>43997</v>
-      </c>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="16"/>
+      <c r="C20" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="48"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="69"/>
-      <c r="B21" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="48"/>
-      <c r="E21" s="43"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="96" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="97" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="94"/>
+      <c r="E21" s="44"/>
       <c r="F21" s="74"/>
       <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
+      <c r="H21" s="25" t="s">
+        <v>97</v>
+      </c>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="69"/>
-      <c r="B22" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="43"/>
+    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="78"/>
+      <c r="B22" s="52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="49"/>
+      <c r="E22" s="44"/>
       <c r="F22" s="74"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="10"/>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="69"/>
-      <c r="B23" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="48"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="79"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="10"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="101" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="83" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="42"/>
+      <c r="F23" s="73">
+        <v>43997</v>
+      </c>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="16"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="69"/>
-      <c r="B24" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="48"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="74">
-        <v>43998</v>
-      </c>
+      <c r="A24" s="77"/>
+      <c r="B24" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="102"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="74"/>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="69"/>
+      <c r="A25" s="77"/>
       <c r="B25" s="53" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="48"/>
-      <c r="E25" s="43"/>
+        <v>86</v>
+      </c>
+      <c r="C25" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="100" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" s="46"/>
       <c r="F25" s="74"/>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="69"/>
-      <c r="B26" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="C26" s="48" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="48"/>
-      <c r="E26" s="43"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="102"/>
+      <c r="D26" s="99"/>
+      <c r="E26" s="46"/>
       <c r="F26" s="74"/>
       <c r="G26" s="25"/>
       <c r="H26" s="25"/>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="70"/>
-      <c r="B27" s="54" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="49"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="79"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="11"/>
-    </row>
-    <row r="28" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="77">
-        <v>43999</v>
-      </c>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="13"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="77"/>
+      <c r="B27" s="53" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="103" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="100" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27" s="46"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="77"/>
+      <c r="B28" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" s="102"/>
+      <c r="D28" s="99"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="71" t="s">
-        <v>65</v>
-      </c>
-      <c r="B29" s="55" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="47" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="47"/>
-      <c r="E29" s="46"/>
+      <c r="A29" s="77"/>
+      <c r="B29" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="C29" s="103" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="100" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="43"/>
       <c r="F29" s="74"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="16"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="73"/>
-      <c r="B30" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="C30" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="49"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="11"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="68" t="s">
-        <v>68</v>
-      </c>
-      <c r="B31" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="47"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="16"/>
+      <c r="A30" s="77"/>
+      <c r="B30" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="102"/>
+      <c r="D30" s="99"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="10"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="77"/>
+      <c r="B31" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="41"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="74">
+        <v>43998</v>
+      </c>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="69"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="53" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" s="48" t="s">
-        <v>48</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="C32" s="41"/>
       <c r="D32" s="48"/>
       <c r="E32" s="43"/>
-      <c r="F32" s="74">
-        <v>44000</v>
-      </c>
+      <c r="F32" s="74"/>
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="70"/>
-      <c r="B33" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="D33" s="49"/>
-      <c r="E33" s="45"/>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="77"/>
+      <c r="B33" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="48"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="43"/>
       <c r="F33" s="74"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="11"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="71" t="s">
-        <v>72</v>
-      </c>
-      <c r="B34" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="47"/>
-      <c r="E34" s="46"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="10"/>
-      <c r="L34" s="6"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="10"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="78"/>
+      <c r="B34" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="11"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="73"/>
-      <c r="B35" s="54" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="49" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="49"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="11"/>
+      <c r="A35" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="27"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="73">
+        <v>43999</v>
+      </c>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="13"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="6"/>
-    </row>
-    <row r="51" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E51" s="5"/>
-      <c r="F51" s="4"/>
+      <c r="A36" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="47"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="74"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="24"/>
+      <c r="I36" s="16"/>
+    </row>
+    <row r="37" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="72"/>
+      <c r="B37" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D37" s="49"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="74"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="11"/>
+    </row>
+    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="76" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="56" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="47"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="24"/>
+      <c r="I38" s="16"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="77"/>
+      <c r="B39" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D39" s="48"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="74">
+        <v>44000</v>
+      </c>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="10"/>
+    </row>
+    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="78"/>
+      <c r="B40" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="49"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="74"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="11"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="47"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="10"/>
+      <c r="L41" s="6"/>
+    </row>
+    <row r="42" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="72"/>
+      <c r="B42" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="49"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="75"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="11"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="6"/>
+    </row>
+    <row r="58" spans="5:6" x14ac:dyDescent="0.25">
+      <c r="E58" s="5"/>
+      <c r="F58" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="33">
+    <mergeCell ref="I12:I17"/>
+    <mergeCell ref="E12:E17"/>
+    <mergeCell ref="G12:G17"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="F39:F42"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="A23:A34"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="I4:I7"/>
     <mergeCell ref="I8:I10"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="F20:F23"/>
-    <mergeCell ref="F24:F27"/>
-    <mergeCell ref="A31:A33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="F28:F31"/>
-    <mergeCell ref="A20:A27"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="F23:F30"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="A12:A17"/>
     <mergeCell ref="A8:A11"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="F18:F22"/>
     <mergeCell ref="F8:F10"/>
     <mergeCell ref="F5:F7"/>
-    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="F12:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1862,6 +2158,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="291a90324d5b7e405cdee1cca19d0e54">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a3d94df2e09d7482e07420c2cba8fd2" ns2:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -2007,22 +2318,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{284D3BA3-53DF-4CD6-A7BE-83F88846B803}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E4F7A1-BDD0-42E0-BF8D-BCF9AB8D9DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E8BDE2A-513D-413D-BAAB-708A15D461DA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2038,21 +2351,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E4F7A1-BDD0-42E0-BF8D-BCF9AB8D9DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{284D3BA3-53DF-4CD6-A7BE-83F88846B803}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Final presentation and schedule clean-up
</commit_message>
<xml_diff>
--- a/Documentation/Stopwatch_Project_Schedule.xlsx
+++ b/Documentation/Stopwatch_Project_Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djste\Documents\GitHub\Time_Travelers_Verilog_Stopwatch\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Files\LTTS\FPGA Training\Projects\Verilog\StopWatch_Verilog\git_repo\Time_Travelers_Verilog_Stopwatch\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5112992E-B82C-4B14-AAC4-DD2C75DD1C55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078988D6-7CB6-4EFE-A1F2-E5F5841A97B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2070" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="144">
   <si>
     <t>Project Stage</t>
   </si>
@@ -347,6 +347,120 @@
   </si>
   <si>
     <t>SWATCH1-109, 110</t>
+  </si>
+  <si>
+    <t>SWATCH1-119</t>
+  </si>
+  <si>
+    <t>SWATCH1-125</t>
+  </si>
+  <si>
+    <t>SWATCH1-126</t>
+  </si>
+  <si>
+    <t>SWATCH1-120</t>
+  </si>
+  <si>
+    <t>SWATCH1-129</t>
+  </si>
+  <si>
+    <t>SWATCH1-128</t>
+  </si>
+  <si>
+    <t>SWATCH1-123</t>
+  </si>
+  <si>
+    <t>SWATCH1-122</t>
+  </si>
+  <si>
+    <t>SWATCH1-121</t>
+  </si>
+  <si>
+    <t>SWATCH1-127</t>
+  </si>
+  <si>
+    <t>SWATCH1-130</t>
+  </si>
+  <si>
+    <t>SWATCH1-146</t>
+  </si>
+  <si>
+    <t>SWATCH1-61</t>
+  </si>
+  <si>
+    <t>SWATCH1-63</t>
+  </si>
+  <si>
+    <t>SWATCH1-62, 131</t>
+  </si>
+  <si>
+    <t>Anonio</t>
+  </si>
+  <si>
+    <t>SWATCH1-65</t>
+  </si>
+  <si>
+    <t>SWATCH1-66</t>
+  </si>
+  <si>
+    <t>SWATCH1-67</t>
+  </si>
+  <si>
+    <t>SWATCH1-135</t>
+  </si>
+  <si>
+    <t>SWATCH1-134</t>
+  </si>
+  <si>
+    <t>Debugging</t>
+  </si>
+  <si>
+    <t>37a6d8e</t>
+  </si>
+  <si>
+    <t>817d09e2</t>
+  </si>
+  <si>
+    <t>4d61a8a8</t>
+  </si>
+  <si>
+    <t>6c32a9f5</t>
+  </si>
+  <si>
+    <t>42c87c45</t>
+  </si>
+  <si>
+    <t>bfba265e</t>
+  </si>
+  <si>
+    <t>34ab6949</t>
+  </si>
+  <si>
+    <t>175786a0</t>
+  </si>
+  <si>
+    <t>10224e37f</t>
+  </si>
+  <si>
+    <t>53969d74</t>
+  </si>
+  <si>
+    <t>082dc411</t>
+  </si>
+  <si>
+    <t>c58cdf0e</t>
+  </si>
+  <si>
+    <t>dc945338</t>
+  </si>
+  <si>
+    <t>ab21ff7a</t>
+  </si>
+  <si>
+    <t>1356c3e7</t>
+  </si>
+  <si>
+    <t>4dfb1490</t>
   </si>
 </sst>
 </file>
@@ -384,7 +498,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,8 +541,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -751,11 +871,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -774,13 +907,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -793,7 +923,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -826,11 +955,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
@@ -864,79 +988,7 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
@@ -947,20 +999,146 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1276,830 +1454,975 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="46" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="34.140625" customWidth="1"/>
-    <col min="11" max="11" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" customWidth="1"/>
+    <col min="10" max="10" width="34.109375" customWidth="1"/>
+    <col min="11" max="11" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="35">
+      <c r="D2" s="38"/>
+      <c r="E2" s="31">
         <v>43985</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="29">
         <v>43985</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="87" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="69" t="s">
         <v>99</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="I2" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79"/>
-      <c r="B3" s="51" t="s">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="80"/>
+      <c r="B3" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="C3" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="48" t="s">
+      <c r="D3" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="62">
+      <c r="E3" s="53">
         <v>43991</v>
       </c>
-      <c r="F3" s="74">
+      <c r="F3" s="77">
         <v>43986</v>
       </c>
-      <c r="G3" s="59" t="s">
+      <c r="G3" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="88"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="19" t="s">
+      <c r="H3" s="70"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="79"/>
-      <c r="B4" s="51" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="80"/>
+      <c r="B4" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="48" t="s">
+      <c r="D4" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="32">
         <v>43986</v>
       </c>
-      <c r="F4" s="74"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="88"/>
-      <c r="I4" s="69" t="s">
+      <c r="F4" s="77"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="107" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
-      <c r="B5" s="51" t="s">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="80"/>
+      <c r="B5" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C5" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="48"/>
-      <c r="E5" s="37">
+      <c r="D5" s="39"/>
+      <c r="E5" s="33">
         <v>43990</v>
       </c>
-      <c r="F5" s="82">
+      <c r="F5" s="83">
         <v>43987</v>
       </c>
-      <c r="G5" s="60" t="s">
+      <c r="G5" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="88"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="21" t="s">
+      <c r="H5" s="70"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="79"/>
-      <c r="B6" s="51" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="80"/>
+      <c r="B6" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="32">
         <v>43987</v>
       </c>
-      <c r="F6" s="82"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="88"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="22" t="s">
+      <c r="F6" s="83"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="72"/>
-      <c r="B7" s="52" t="s">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="76"/>
+      <c r="B7" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="38">
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="34">
         <v>43990</v>
       </c>
-      <c r="F7" s="82"/>
-      <c r="G7" s="61" t="s">
+      <c r="F7" s="83"/>
+      <c r="G7" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="89"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="11"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="76" t="s">
+      <c r="H7" s="71"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="47" t="s">
+      <c r="C8" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="35">
         <v>43987</v>
       </c>
-      <c r="F8" s="73">
+      <c r="F8" s="79">
         <v>43990</v>
       </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="68" t="s">
+      <c r="G8" s="21"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="106" t="s">
         <v>74</v>
       </c>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="77"/>
-      <c r="B9" s="53" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="73"/>
+      <c r="B9" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="81"/>
-      <c r="E9" s="40">
+      <c r="D9" s="82"/>
+      <c r="E9" s="36">
         <v>43987</v>
       </c>
-      <c r="F9" s="74"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="25" t="s">
+      <c r="F9" s="77"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="I9" s="69"/>
+      <c r="I9" s="107"/>
       <c r="J9" s="6"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="77"/>
-      <c r="B10" s="53" t="s">
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="73"/>
+      <c r="B10" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="48"/>
-      <c r="E10" s="67">
+      <c r="D10" s="39"/>
+      <c r="E10" s="58">
         <v>43990</v>
       </c>
-      <c r="F10" s="74"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="25" t="s">
+      <c r="F10" s="77"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="I10" s="69"/>
+      <c r="I10" s="107"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="78"/>
-      <c r="B11" s="54" t="s">
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="74"/>
+      <c r="B11" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="49"/>
-      <c r="E11" s="66">
+      <c r="D11" s="40"/>
+      <c r="E11" s="57">
         <v>43993</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F11" s="30">
         <v>43992</v>
       </c>
-      <c r="G11" s="63" t="s">
+      <c r="G11" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="H11" s="26" t="s">
+      <c r="H11" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="I11" s="11"/>
+      <c r="I11" s="109"/>
       <c r="J11" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="71" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="47" t="s">
+      <c r="C12" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="38" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="90">
+      <c r="E12" s="66">
         <v>43994</v>
       </c>
-      <c r="F12" s="73">
+      <c r="F12" s="79">
         <v>43993</v>
       </c>
-      <c r="G12" s="87" t="s">
+      <c r="G12" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="I12" s="86" t="s">
+      <c r="I12" s="110" t="s">
         <v>75</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="79"/>
-      <c r="B13" s="95" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="80"/>
+      <c r="B13" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="48" t="s">
+      <c r="C13" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="E13" s="91"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="25" t="s">
+      <c r="E13" s="67"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="91"/>
+      <c r="H13" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="I13" s="84"/>
+      <c r="I13" s="111"/>
       <c r="J13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="79"/>
-      <c r="B14" s="53" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="80"/>
+      <c r="B14" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="91"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="25" t="s">
+      <c r="E14" s="67"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="I14" s="84"/>
+      <c r="I14" s="111"/>
       <c r="J14" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="79"/>
-      <c r="B15" s="53" t="s">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="80"/>
+      <c r="B15" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="94" t="s">
+      <c r="C15" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="94" t="s">
+      <c r="D15" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="E15" s="91"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="25" t="s">
+      <c r="E15" s="67"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="I15" s="84"/>
+      <c r="I15" s="111"/>
       <c r="J15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="79"/>
-      <c r="B16" s="93" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="80"/>
+      <c r="B16" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="94" t="s">
+      <c r="C16" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="94" t="s">
+      <c r="D16" s="61" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="91"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="88"/>
-      <c r="H16" s="25" t="s">
+      <c r="E16" s="67"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="91"/>
+      <c r="H16" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="I16" s="84"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="72"/>
-      <c r="B17" s="54" t="s">
+      <c r="I16" s="111"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="76"/>
+      <c r="B17" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="92"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="26" t="s">
+      <c r="E17" s="68"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="I17" s="85"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="76" t="s">
+      <c r="I17" s="112"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="73">
+      <c r="D18" s="38"/>
+      <c r="E18" s="93">
         <v>43994</v>
       </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24" t="s">
+      <c r="F18" s="79">
+        <v>43994</v>
+      </c>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="I18" s="16"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="77"/>
-      <c r="B19" s="51" t="s">
+      <c r="I18" s="102" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="73"/>
+      <c r="B19" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="48"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25" t="s">
+      <c r="D19" s="39"/>
+      <c r="E19" s="94">
+        <v>43994</v>
+      </c>
+      <c r="F19" s="77"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="I19" s="10"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="77"/>
-      <c r="B20" s="51" t="s">
+      <c r="I19" s="103" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="73"/>
+      <c r="B20" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="48"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25" t="s">
+      <c r="D20" s="39"/>
+      <c r="E20" s="53">
+        <v>43997</v>
+      </c>
+      <c r="F20" s="77"/>
+      <c r="G20" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="H20" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="I20" s="10"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="77"/>
-      <c r="B21" s="96" t="s">
+      <c r="I20" s="103" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="73"/>
+      <c r="B21" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="97" t="s">
+      <c r="C21" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="94"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25" t="s">
+      <c r="D21" s="61"/>
+      <c r="E21" s="95">
+        <v>43994</v>
+      </c>
+      <c r="F21" s="77"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="I21" s="10"/>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="78"/>
-      <c r="B22" s="52" t="s">
+      <c r="I21" s="103" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="74"/>
+      <c r="B22" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="58" t="s">
+      <c r="C22" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="49"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26" t="s">
+      <c r="D22" s="40"/>
+      <c r="E22" s="95">
+        <v>43994</v>
+      </c>
+      <c r="F22" s="77"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="76" t="s">
+      <c r="I22" s="104" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="C23" s="101" t="s">
+      <c r="C23" s="84" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="83" t="s">
+      <c r="D23" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="73">
+      <c r="E23" s="93">
         <v>43997</v>
       </c>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="16"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="77"/>
+      <c r="F23" s="79">
+        <v>43997</v>
+      </c>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="I23" s="102" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="73"/>
       <c r="B24" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C24" s="102"/>
-      <c r="D24" s="99"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="10"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="77"/>
-      <c r="B25" s="53" t="s">
+      <c r="C24" s="86"/>
+      <c r="D24" s="87"/>
+      <c r="E24" s="97">
+        <v>43998</v>
+      </c>
+      <c r="F24" s="77"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="I24" s="103" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="73"/>
+      <c r="B25" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="C25" s="103" t="s">
+      <c r="C25" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="100" t="s">
+      <c r="D25" s="89" t="s">
         <v>76</v>
       </c>
-      <c r="E25" s="46"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="10"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="77"/>
+      <c r="E25" s="96">
+        <v>43997</v>
+      </c>
+      <c r="F25" s="77"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" s="103" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="73"/>
       <c r="B26" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="102"/>
-      <c r="D26" s="99"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="10"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="77"/>
-      <c r="B27" s="53" t="s">
+      <c r="C26" s="86"/>
+      <c r="D26" s="87"/>
+      <c r="E26" s="97">
+        <v>43998</v>
+      </c>
+      <c r="F26" s="77"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="I26" s="103" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="73"/>
+      <c r="B27" s="44" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="103" t="s">
+      <c r="C27" s="88" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="100" t="s">
+      <c r="D27" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="46"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="10"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="77"/>
+      <c r="E27" s="96">
+        <v>43997</v>
+      </c>
+      <c r="F27" s="77"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="I27" s="103" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="73"/>
       <c r="B28" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="102"/>
-      <c r="D28" s="99"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="10"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="77"/>
-      <c r="B29" s="53" t="s">
+      <c r="C28" s="86"/>
+      <c r="D28" s="87"/>
+      <c r="E28" s="53">
+        <v>43998</v>
+      </c>
+      <c r="F28" s="77"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="I28" s="103" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="73"/>
+      <c r="B29" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="C29" s="103" t="s">
+      <c r="C29" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="D29" s="100" t="s">
+      <c r="D29" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="E29" s="43"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="10"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="77"/>
+      <c r="E29" s="94">
+        <v>43997</v>
+      </c>
+      <c r="F29" s="77"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="I29" s="103" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="73"/>
       <c r="B30" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="102"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="10"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="77"/>
-      <c r="B31" s="53" t="s">
+      <c r="C30" s="86"/>
+      <c r="D30" s="87"/>
+      <c r="E30" s="53">
+        <v>43998</v>
+      </c>
+      <c r="F30" s="78"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="I30" s="103" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="73"/>
+      <c r="B31" s="44" t="s">
         <v>56</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="48"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="74">
+      <c r="C31" s="37"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="94">
         <v>43998</v>
       </c>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="10"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="77"/>
-      <c r="B32" s="53" t="s">
+      <c r="F31" s="77">
+        <v>43998</v>
+      </c>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="I31" s="103" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="73"/>
+      <c r="B32" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="48"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="10"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="77"/>
-      <c r="B33" s="53" t="s">
+      <c r="C32" s="37"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="94">
+        <v>43998</v>
+      </c>
+      <c r="F32" s="77"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="I32" s="103" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="73"/>
+      <c r="B33" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="43"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="10"/>
-    </row>
-    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="78"/>
-      <c r="B34" s="54" t="s">
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="94">
+        <v>43998</v>
+      </c>
+      <c r="F33" s="77"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="I33" s="103" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="74"/>
+      <c r="B34" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="11"/>
-    </row>
-    <row r="35" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="32" t="s">
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="98">
+        <v>43998</v>
+      </c>
+      <c r="F34" s="78"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="I34" s="104" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="73">
+      <c r="C35" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="24"/>
+      <c r="E35" s="100">
         <v>43999</v>
       </c>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="13"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="71" t="s">
+      <c r="F35" s="79">
+        <v>43999</v>
+      </c>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="I35" s="105" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="55" t="s">
+      <c r="B36" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="D36" s="47"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="16"/>
-    </row>
-    <row r="37" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="72"/>
-      <c r="B37" s="52" t="s">
+      <c r="D36" s="38" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="96">
+        <v>43999</v>
+      </c>
+      <c r="F36" s="77"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="I36" s="102" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="76"/>
+      <c r="B37" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="49" t="s">
+      <c r="C37" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="40"/>
+      <c r="E37" s="101">
+        <v>44000</v>
+      </c>
+      <c r="F37" s="77"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="I37" s="104" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="72" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" s="38"/>
+      <c r="E38" s="96">
+        <v>43999</v>
+      </c>
+      <c r="F38" s="78"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="I38" s="102" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="73"/>
+      <c r="B39" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="74"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="26"/>
-      <c r="I37" s="11"/>
-    </row>
-    <row r="38" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="76" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="47" t="s">
+      <c r="D39" s="39"/>
+      <c r="E39" s="94">
+        <v>44000</v>
+      </c>
+      <c r="F39" s="79">
+        <v>44000</v>
+      </c>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="I39" s="103" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="74"/>
+      <c r="B40" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="C40" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" s="40"/>
+      <c r="E40" s="98">
+        <v>44000</v>
+      </c>
+      <c r="F40" s="77"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="I40" s="104" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="75" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="47"/>
-      <c r="E38" s="46"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="16"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="77"/>
-      <c r="B39" s="53" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" s="48" t="s">
-        <v>45</v>
-      </c>
-      <c r="D39" s="48"/>
-      <c r="E39" s="43"/>
-      <c r="F39" s="74">
+      <c r="D41" s="38"/>
+      <c r="E41" s="96">
         <v>44000</v>
       </c>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="10"/>
-    </row>
-    <row r="40" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="78"/>
-      <c r="B40" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="D40" s="49"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="74"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="11"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="71" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="55" t="s">
-        <v>69</v>
-      </c>
-      <c r="C41" s="47" t="s">
+      <c r="F41" s="99"/>
+      <c r="G41" s="22"/>
+      <c r="H41" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="I41" s="103" t="s">
+        <v>143</v>
+      </c>
+      <c r="L41" s="6"/>
+    </row>
+    <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="76"/>
+      <c r="B42" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="47"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="74"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="10"/>
-      <c r="L41" s="6"/>
-    </row>
-    <row r="42" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="72"/>
-      <c r="B42" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="49"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="75"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="11"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D42" s="40"/>
+      <c r="E42" s="98">
+        <v>44001</v>
+      </c>
+      <c r="F42" s="59">
+        <v>44001</v>
+      </c>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="I42" s="10"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="9"/>
@@ -2109,22 +2432,19 @@
       <c r="H43" s="6"/>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B44" s="6"/>
     </row>
-    <row r="58" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E58" s="5"/>
       <c r="F58" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="I12:I17"/>
-    <mergeCell ref="E12:E17"/>
-    <mergeCell ref="G12:G17"/>
-    <mergeCell ref="H2:H7"/>
-    <mergeCell ref="A38:A40"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="F12:F17"/>
+    <mergeCell ref="F39:F41"/>
     <mergeCell ref="A41:A42"/>
-    <mergeCell ref="F39:F42"/>
     <mergeCell ref="F35:F38"/>
     <mergeCell ref="A23:A34"/>
     <mergeCell ref="D23:D24"/>
@@ -2135,12 +2455,17 @@
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="F23:F30"/>
+    <mergeCell ref="F31:F34"/>
+    <mergeCell ref="I12:I17"/>
+    <mergeCell ref="E12:E17"/>
+    <mergeCell ref="G12:G17"/>
+    <mergeCell ref="H2:H7"/>
+    <mergeCell ref="A38:A40"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="I4:I7"/>
     <mergeCell ref="I8:I10"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="F23:F30"/>
-    <mergeCell ref="F31:F34"/>
     <mergeCell ref="A18:A22"/>
     <mergeCell ref="A12:A17"/>
     <mergeCell ref="A8:A11"/>
@@ -2149,8 +2474,6 @@
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="F18:F22"/>
     <mergeCell ref="F8:F10"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="F12:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2158,21 +2481,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="291a90324d5b7e405cdee1cca19d0e54">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1a3d94df2e09d7482e07420c2cba8fd2" ns2:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -2318,24 +2626,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{284D3BA3-53DF-4CD6-A7BE-83F88846B803}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E4F7A1-BDD0-42E0-BF8D-BCF9AB8D9DFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E8BDE2A-513D-413D-BAAB-708A15D461DA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2351,4 +2657,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E4F7A1-BDD0-42E0-BF8D-BCF9AB8D9DFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{284D3BA3-53DF-4CD6-A7BE-83F88846B803}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>